<commit_message>
make like of college
</commit_message>
<xml_diff>
--- a/PartnerData/excel/Humanity.xlsx
+++ b/PartnerData/excel/Humanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jahyeon_gu/Partnermap/PartnerData/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6898B1FE-FB5F-D14E-B851-525E6513B921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02312E0-F281-3B41-8D41-2667DDB890F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,28 +515,8 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="나눔고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="-apple-system"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,7 +556,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -598,28 +578,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -961,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="138" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1005,7 +970,7 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1088,7 +1053,7 @@
       <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="9" t="s">
         <v>122</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1108,7 +1073,7 @@
       <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>115</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1188,7 +1153,7 @@
       <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="9" t="s">
         <v>121</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1208,7 +1173,7 @@
       <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="9" t="s">
         <v>109</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1225,7 +1190,7 @@
       <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1248,7 +1213,7 @@
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="9" t="s">
         <v>120</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -1265,10 +1230,10 @@
       <c r="C15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="9" t="s">
         <v>119</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -1288,7 +1253,7 @@
       <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1325,10 +1290,10 @@
       <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="9" t="s">
         <v>117</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1362,7 +1327,7 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1382,7 +1347,7 @@
       <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>104</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1402,7 +1367,7 @@
       <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1425,7 +1390,7 @@
       <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="9" t="s">
         <v>116</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -1465,7 +1430,7 @@
       <c r="D25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="9" t="s">
         <v>115</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -1505,7 +1470,7 @@
       <c r="D27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="9" t="s">
         <v>114</v>
       </c>
       <c r="F27" s="6" t="s">
@@ -1525,7 +1490,7 @@
       <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="9" t="s">
         <v>112</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -1545,7 +1510,7 @@
       <c r="D29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="9" t="s">
         <v>113</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -1562,10 +1527,10 @@
       <c r="C30" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="9" t="s">
         <v>111</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -1605,116 +1570,12 @@
       <c r="D32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="16">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" ht="21">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="14"/>
-    </row>
-    <row r="35" spans="1:5" ht="16">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" ht="16">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" ht="16">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" ht="16">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" ht="16">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" ht="16">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" ht="16">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:5" ht="16">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:5" ht="16">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" ht="16">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" ht="16">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" ht="16">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" ht="16">
-      <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>